<commit_message>
LLL H8D support added, Updated MessageBopx Title to Disk Image Utility, Added IMD to IMG conversion, Corrected program error when adding files to image
</commit_message>
<xml_diff>
--- a/DiskUtility/Skew Table.xlsx
+++ b/DiskUtility/Skew Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\Github\DiskUtility\DiskUtility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dev\Github\DiskImageUtility\DiskUtility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15E1857-0D74-4866-A250-699312D7B942}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B232DA4E-914C-409B-9DA7-11614A7D6398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29160" yWindow="2145" windowWidth="27240" windowHeight="13275" activeTab="3" xr2:uid="{DD7A5C08-DCA6-4B6E-BD23-734986915BC7}"/>
+    <workbookView xWindow="31995" yWindow="1725" windowWidth="25470" windowHeight="11835" activeTab="3" xr2:uid="{DD7A5C08-DCA6-4B6E-BD23-734986915BC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Skew" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="251">
   <si>
     <t>Skew</t>
   </si>
@@ -791,6 +791,9 @@
   </si>
   <si>
     <t>SPT (128 bytes)</t>
+  </si>
+  <si>
+    <t>LLL Format</t>
   </si>
 </sst>
 </file>
@@ -864,7 +867,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -922,12 +925,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1036,6 +1050,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4991,10 +5015,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B79399-9BB6-4B97-BE36-8FE45530B141}">
-  <dimension ref="A2:AO43"/>
+  <dimension ref="A2:AO46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G6" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="N6" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5300,7 +5324,7 @@
         <v>2</v>
       </c>
       <c r="X8" s="43">
-        <f t="shared" ref="X8:X16" si="1">T8*U8*V8*W8</f>
+        <f t="shared" ref="X8:X18" si="1">T8*U8*V8*W8</f>
         <v>819200</v>
       </c>
       <c r="Y8" s="19" t="s">
@@ -5319,7 +5343,7 @@
         <v>2048</v>
       </c>
       <c r="AD8" s="42">
-        <f t="shared" ref="AD8:AD16" si="2">X8/AC8</f>
+        <f t="shared" ref="AD8:AD17" si="2">X8/AC8</f>
         <v>400</v>
       </c>
       <c r="AE8" s="42">
@@ -6101,642 +6125,720 @@
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
-      <c r="Y17" s="8"/>
-    </row>
-    <row r="18" spans="1:38" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="R17" t="s">
+        <v>250</v>
+      </c>
+      <c r="S17" s="46"/>
+      <c r="T17" s="51">
+        <v>10</v>
+      </c>
+      <c r="U17" s="51">
+        <v>256</v>
+      </c>
+      <c r="V17" s="51">
+        <v>40</v>
+      </c>
+      <c r="W17" s="51">
+        <v>2</v>
+      </c>
+      <c r="X17" s="47">
+        <f t="shared" si="1"/>
+        <v>204800</v>
+      </c>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="49"/>
+      <c r="AA17" s="50"/>
+      <c r="AB17" s="7">
+        <v>7680</v>
+      </c>
+      <c r="AC17" s="7">
+        <v>2048</v>
+      </c>
+      <c r="AD17" s="42">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="AE17" s="42"/>
+      <c r="AF17" s="7">
+        <v>8192</v>
+      </c>
+      <c r="AI17" s="40"/>
+      <c r="AJ17" s="40"/>
+      <c r="AK17" s="40"/>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="R18" t="s">
+        <v>250</v>
+      </c>
+      <c r="S18" s="46"/>
+      <c r="T18" s="51">
+        <v>10</v>
+      </c>
+      <c r="U18" s="51">
+        <v>256</v>
+      </c>
+      <c r="V18" s="51">
+        <v>80</v>
+      </c>
+      <c r="W18" s="51">
+        <v>2</v>
+      </c>
+      <c r="X18" s="47">
+        <f t="shared" si="1"/>
+        <v>409600</v>
+      </c>
+      <c r="Y18" s="48"/>
+      <c r="Z18" s="49"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="7">
+        <v>7680</v>
+      </c>
+      <c r="AC18" s="7">
+        <v>2048</v>
+      </c>
+      <c r="AD18" s="42">
+        <f t="shared" ref="AD18" si="5">X18/AC18</f>
+        <v>200</v>
+      </c>
+      <c r="AE18" s="42"/>
+      <c r="AF18" s="7">
+        <v>8192</v>
+      </c>
+      <c r="AI18" s="40"/>
+      <c r="AJ18" s="40"/>
+      <c r="AK18" s="40"/>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="S19" s="46"/>
+      <c r="T19" s="46"/>
+      <c r="U19" s="46"/>
+      <c r="V19" s="46"/>
+      <c r="W19" s="46"/>
+      <c r="X19" s="47"/>
+      <c r="Y19" s="48"/>
+      <c r="Z19" s="49"/>
+      <c r="AA19" s="50"/>
+      <c r="AB19" s="7"/>
+      <c r="AD19" s="42"/>
+      <c r="AE19" s="42"/>
+      <c r="AF19" s="7"/>
+      <c r="AI19" s="40"/>
+      <c r="AJ19" s="40"/>
+      <c r="AK19" s="40"/>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="Y20" s="8"/>
+    </row>
+    <row r="21" spans="1:38" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H21" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I21" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="J18" s="7" t="s">
+      <c r="J21" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="K21" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="L21" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="M21" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="N18" s="14" t="s">
+      <c r="N21" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="O18" s="7" t="s">
+      <c r="O21" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="P18" s="7" t="s">
+      <c r="P21" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="Q18" s="14"/>
-      <c r="T18" s="16" t="s">
+      <c r="Q21" s="14"/>
+      <c r="T21" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="U18" s="16" t="s">
+      <c r="U21" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="V18" s="16" t="s">
+      <c r="V21" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="W18" s="16" t="s">
+      <c r="W21" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="X18" s="16" t="s">
+      <c r="X21" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="Y18" s="16" t="s">
+      <c r="Y21" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="Z18" s="17" t="s">
+      <c r="Z21" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="AA18" s="17" t="s">
+      <c r="AA21" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
         <v>0</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>102</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
         <v>27</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D22" t="s">
         <v>33</v>
       </c>
-      <c r="E19">
+      <c r="E22">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F22" t="s">
         <v>22</v>
       </c>
-      <c r="G19">
+      <c r="G22">
         <v>1</v>
       </c>
-      <c r="H19">
+      <c r="H22">
         <v>8</v>
       </c>
-      <c r="I19">
+      <c r="I22">
         <v>512</v>
       </c>
-      <c r="J19">
+      <c r="J22">
         <v>40</v>
       </c>
-      <c r="K19">
+      <c r="K22">
         <v>2</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L22" t="s">
         <v>107</v>
       </c>
-      <c r="M19">
+      <c r="M22">
         <v>1</v>
       </c>
-      <c r="N19" s="8" t="s">
+      <c r="N22" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O22" t="s">
         <v>112</v>
       </c>
-      <c r="P19" s="11">
-        <f>H19*I19*J19*K19</f>
+      <c r="P22" s="11">
+        <f>H22*I22*J22*K22</f>
         <v>327680</v>
       </c>
-      <c r="Q19" s="8" t="s">
+      <c r="Q22" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="T19" s="31" t="s">
+      <c r="T22" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="U19" s="31">
+      <c r="U22" s="31">
         <v>8</v>
       </c>
-      <c r="V19" s="31">
+      <c r="V22" s="31">
         <v>512</v>
       </c>
-      <c r="W19" s="31">
+      <c r="W22" s="31">
         <v>40</v>
       </c>
-      <c r="X19" s="31">
+      <c r="X22" s="31">
         <v>2</v>
       </c>
-      <c r="Y19" s="32">
-        <f t="shared" ref="Y19:Y22" si="5">U19*V19*W19*X19</f>
+      <c r="Y22" s="32">
+        <f t="shared" ref="Y22:Y25" si="6">U22*V22*W22*X22</f>
         <v>327680</v>
       </c>
-      <c r="Z19" s="18" t="s">
+      <c r="Z22" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="AA19" s="33" t="s">
+      <c r="AA22" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="AG19">
+      <c r="AG22">
         <f>9*512</f>
         <v>4608</v>
       </c>
-      <c r="AH19" t="str">
-        <f>DEC2HEX(AG19)</f>
+      <c r="AH22" t="str">
+        <f>DEC2HEX(AG22)</f>
         <v>1200</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>103</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D23" t="s">
         <v>33</v>
       </c>
-      <c r="E20">
+      <c r="E23">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F23" t="s">
         <v>22</v>
       </c>
-      <c r="G20">
+      <c r="G23">
         <v>1</v>
       </c>
-      <c r="H20">
+      <c r="H23">
         <v>9</v>
       </c>
-      <c r="I20">
+      <c r="I23">
         <v>512</v>
       </c>
-      <c r="J20">
+      <c r="J23">
         <v>40</v>
       </c>
-      <c r="K20">
+      <c r="K23">
         <v>2</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L23" t="s">
         <v>107</v>
       </c>
-      <c r="M20">
+      <c r="M23">
         <v>2</v>
       </c>
-      <c r="N20" s="8" t="s">
+      <c r="N23" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O23" t="s">
         <v>113</v>
       </c>
-      <c r="P20" s="11">
-        <f t="shared" ref="P20:P22" si="6">H20*I20*J20*K20</f>
+      <c r="P23" s="11">
+        <f t="shared" ref="P23:P25" si="7">H23*I23*J23*K23</f>
         <v>368640</v>
       </c>
-      <c r="Q20" s="8" t="s">
+      <c r="Q23" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="T20" s="31" t="s">
+      <c r="T23" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="U20" s="31">
+      <c r="U23" s="31">
         <v>9</v>
       </c>
-      <c r="V20" s="31">
+      <c r="V23" s="31">
         <v>512</v>
       </c>
-      <c r="W20" s="31">
+      <c r="W23" s="31">
         <v>40</v>
       </c>
-      <c r="X20" s="31">
+      <c r="X23" s="31">
         <v>2</v>
       </c>
-      <c r="Y20" s="32">
-        <f t="shared" si="5"/>
+      <c r="Y23" s="32">
+        <f t="shared" si="6"/>
         <v>368640</v>
       </c>
-      <c r="Z20" s="18" t="s">
+      <c r="Z23" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="AA20" s="33" t="s">
+      <c r="AA23" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="AG20">
-        <f>AG$19+AG19</f>
+      <c r="AG23">
+        <f>AG$22+AG22</f>
         <v>9216</v>
       </c>
-      <c r="AH20" t="str">
-        <f>DEC2HEX(AG20)</f>
+      <c r="AH23" t="str">
+        <f>DEC2HEX(AG23)</f>
         <v>2400</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A24" s="12">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B24" t="s">
         <v>104</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>27</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="E21">
+      <c r="E24">
         <v>1</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F24" t="s">
         <v>22</v>
       </c>
-      <c r="G21">
+      <c r="G24">
         <v>1</v>
       </c>
-      <c r="H21">
+      <c r="H24">
         <v>8</v>
       </c>
-      <c r="I21">
+      <c r="I24">
         <v>512</v>
       </c>
-      <c r="J21">
+      <c r="J24">
         <v>80</v>
       </c>
-      <c r="K21">
+      <c r="K24">
         <v>2</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L24" t="s">
         <v>107</v>
       </c>
-      <c r="M21">
+      <c r="M24">
         <v>2</v>
       </c>
-      <c r="N21" s="8" t="s">
+      <c r="N24" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O24" t="s">
         <v>115</v>
       </c>
-      <c r="P21" s="11">
+      <c r="P24" s="11">
+        <f t="shared" si="7"/>
+        <v>655360</v>
+      </c>
+      <c r="Q24" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="T24" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="U24" s="31">
+        <v>8</v>
+      </c>
+      <c r="V24" s="31">
+        <v>512</v>
+      </c>
+      <c r="W24" s="31">
+        <v>80</v>
+      </c>
+      <c r="X24" s="31">
+        <v>2</v>
+      </c>
+      <c r="Y24" s="32">
         <f t="shared" si="6"/>
         <v>655360</v>
       </c>
-      <c r="Q21" s="8" t="s">
+      <c r="Z24" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="T21" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="U21" s="31">
+      <c r="AA24" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG24">
+        <f>AG$22+AG23</f>
+        <v>13824</v>
+      </c>
+      <c r="AH24" t="str">
+        <f>DEC2HEX(AG24)</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" t="s">
+        <v>106</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
         <v>8</v>
       </c>
-      <c r="V21" s="31">
-        <v>512</v>
-      </c>
-      <c r="W21" s="31">
+      <c r="I25">
+        <v>1024</v>
+      </c>
+      <c r="J25">
+        <v>77</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+      <c r="L25" t="s">
+        <v>108</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="O25" t="s">
+        <v>114</v>
+      </c>
+      <c r="P25" s="11">
+        <f t="shared" si="7"/>
+        <v>1261568</v>
+      </c>
+      <c r="Q25" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="X21" s="31">
+      <c r="T25" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="U25" s="31">
+        <v>8</v>
+      </c>
+      <c r="V25" s="31">
+        <v>1024</v>
+      </c>
+      <c r="W25" s="31">
+        <v>77</v>
+      </c>
+      <c r="X25" s="31">
         <v>2</v>
       </c>
-      <c r="Y21" s="32">
-        <f t="shared" si="5"/>
-        <v>655360</v>
-      </c>
-      <c r="Z21" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA21" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="AG21">
-        <f>AG$19+AG20</f>
-        <v>13824</v>
-      </c>
-      <c r="AH21" t="str">
-        <f>DEC2HEX(AG21)</f>
-        <v>3600</v>
-      </c>
-    </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A22" s="13">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" t="s">
-        <v>106</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>8</v>
-      </c>
-      <c r="I22">
-        <v>1024</v>
-      </c>
-      <c r="J22">
-        <v>77</v>
-      </c>
-      <c r="K22">
-        <v>2</v>
-      </c>
-      <c r="L22" t="s">
-        <v>108</v>
-      </c>
-      <c r="M22">
-        <v>2</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="O22" t="s">
-        <v>114</v>
-      </c>
-      <c r="P22" s="11">
+      <c r="Y25" s="32">
         <f t="shared" si="6"/>
         <v>1261568</v>
       </c>
-      <c r="Q22" s="8" t="s">
+      <c r="Z25" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="T22" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="U22" s="31">
-        <v>8</v>
-      </c>
-      <c r="V22" s="31">
-        <v>1024</v>
-      </c>
-      <c r="W22" s="31">
-        <v>77</v>
-      </c>
-      <c r="X22" s="31">
+      <c r="AA25" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG25">
+        <f>AG$22+AG24</f>
+        <v>18432</v>
+      </c>
+      <c r="AH25" t="str">
+        <f>DEC2HEX(AG25)</f>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>18</v>
+      </c>
+      <c r="I26">
+        <v>512</v>
+      </c>
+      <c r="J26">
+        <v>80</v>
+      </c>
+      <c r="K26">
         <v>2</v>
       </c>
-      <c r="Y22" s="32">
-        <f t="shared" si="5"/>
-        <v>1261568</v>
-      </c>
-      <c r="Z22" s="18" t="s">
+      <c r="L26" t="s">
+        <v>107</v>
+      </c>
+      <c r="M26">
+        <v>9</v>
+      </c>
+      <c r="N26" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="O26" t="s">
+        <v>174</v>
+      </c>
+      <c r="P26" s="11">
+        <f>H26*I26*J26*K26</f>
+        <v>1474560</v>
+      </c>
+      <c r="Q26" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="AA22" s="33" t="s">
+      <c r="T26" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="U26" s="31">
+        <v>18</v>
+      </c>
+      <c r="V26" s="31">
+        <v>512</v>
+      </c>
+      <c r="W26" s="31">
+        <v>80</v>
+      </c>
+      <c r="X26" s="31">
+        <v>2</v>
+      </c>
+      <c r="Y26" s="32">
+        <f t="shared" ref="Y26" si="8">U26*V26*W26*X26</f>
+        <v>1474560</v>
+      </c>
+      <c r="Z26" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA26" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="AG22">
-        <f>AG$19+AG21</f>
-        <v>18432</v>
-      </c>
-      <c r="AH22" t="str">
-        <f>DEC2HEX(AG22)</f>
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="H23">
-        <v>18</v>
-      </c>
-      <c r="I23">
-        <v>512</v>
-      </c>
-      <c r="J23">
-        <v>80</v>
-      </c>
-      <c r="K23">
-        <v>2</v>
-      </c>
-      <c r="L23" t="s">
-        <v>107</v>
-      </c>
-      <c r="M23">
-        <v>9</v>
-      </c>
-      <c r="N23" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="O23" t="s">
-        <v>174</v>
-      </c>
-      <c r="P23" s="11">
-        <f>H23*I23*J23*K23</f>
-        <v>1474560</v>
-      </c>
-      <c r="Q23" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="T23" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="U23" s="31">
-        <v>18</v>
-      </c>
-      <c r="V23" s="31">
-        <v>512</v>
-      </c>
-      <c r="W23" s="31">
-        <v>80</v>
-      </c>
-      <c r="X23" s="31">
-        <v>2</v>
-      </c>
-      <c r="Y23" s="32">
-        <f t="shared" ref="Y23" si="7">U23*V23*W23*X23</f>
-        <v>1474560</v>
-      </c>
-      <c r="Z23" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA23" s="33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AJ24" t="s">
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AJ27" t="s">
         <v>223</v>
       </c>
-      <c r="AK24" t="s">
+      <c r="AK27" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AH25" t="s">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AH28" t="s">
         <v>239</v>
       </c>
-      <c r="AI25" t="s">
+      <c r="AI28" t="s">
         <v>240</v>
       </c>
-      <c r="AJ25" t="s">
+      <c r="AJ28" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AH26">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AH29">
         <v>72</v>
       </c>
-      <c r="AI26" s="8">
+      <c r="AI29" s="8">
         <v>48</v>
       </c>
-      <c r="AJ26" s="44">
+      <c r="AJ29" s="44">
         <v>20</v>
       </c>
-      <c r="AK26">
+      <c r="AK29">
         <v>32</v>
       </c>
-      <c r="AL26" t="s">
+      <c r="AL29" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AI27" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ27" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AI28" s="8">
-        <v>5</v>
-      </c>
-      <c r="AJ28" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AI29" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="AJ29" s="8" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="AI30" s="8">
         <v>0</v>
       </c>
-      <c r="AJ30" s="8">
+      <c r="AJ30" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AI31" s="8">
+        <v>5</v>
+      </c>
+      <c r="AJ31" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AI32" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ32" s="8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="33" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI33" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ33" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AI31" s="8" t="s">
+    <row r="34" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI34" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="AJ31" s="44" t="s">
+      <c r="AJ34" s="44" t="s">
         <v>243</v>
       </c>
-      <c r="AK31">
+      <c r="AK34">
         <v>155</v>
       </c>
-      <c r="AL31" t="s">
+      <c r="AL34" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AI32" s="8">
+    <row r="35" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI35" s="8">
         <v>6</v>
       </c>
-      <c r="AJ32" s="45">
+      <c r="AJ35" s="45">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI33" s="8" t="s">
+    <row r="36" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI36" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="AJ33" s="44" t="s">
+      <c r="AJ36" s="44" t="s">
         <v>82</v>
       </c>
-      <c r="AK33">
+      <c r="AK36">
         <v>255</v>
       </c>
-      <c r="AL33" t="s">
+      <c r="AL36" t="s">
         <v>247</v>
-      </c>
-    </row>
-    <row r="34" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI34" s="8">
-        <v>3</v>
-      </c>
-      <c r="AJ34" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI35" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AJ35" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI36" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ36" s="8">
-        <v>0</v>
       </c>
     </row>
     <row r="37" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI37" s="8">
+        <v>3</v>
+      </c>
+      <c r="AJ37" s="45">
         <v>0</v>
       </c>
-      <c r="AJ37" s="8">
-        <v>40</v>
-      </c>
     </row>
     <row r="38" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI38" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ38" s="8">
-        <v>0</v>
+      <c r="AI38" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="AJ38" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="35:38" x14ac:dyDescent="0.25">
       <c r="AI39" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ39" s="8">
-        <v>2</v>
-      </c>
-      <c r="AL39" t="s">
-        <v>248</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="35:38" x14ac:dyDescent="0.25">
@@ -6744,20 +6846,47 @@
         <v>0</v>
       </c>
       <c r="AJ40" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI41" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI41" s="8"/>
-      <c r="AJ41" s="8"/>
+      <c r="AJ41" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI42" s="8"/>
-      <c r="AJ42" s="8"/>
+      <c r="AI42" s="8">
+        <v>1</v>
+      </c>
+      <c r="AJ42" s="8">
+        <v>2</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="43" spans="35:38" x14ac:dyDescent="0.25">
-      <c r="AI43" s="8"/>
-      <c r="AJ43" s="8"/>
+      <c r="AI43" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ43" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI44" s="8"/>
+      <c r="AJ44" s="8"/>
+    </row>
+    <row r="45" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI45" s="8"/>
+      <c r="AJ45" s="8"/>
+    </row>
+    <row r="46" spans="35:38" x14ac:dyDescent="0.25">
+      <c r="AI46" s="8"/>
+      <c r="AJ46" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>